<commit_message>
GUI Update + analyze_cube added
</commit_message>
<xml_diff>
--- a/Блок-схема.xlsx
+++ b/Блок-схема.xlsx
@@ -64,14 +64,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>174810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165285</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -82,8 +82,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4705350" y="914400"/>
-          <a:ext cx="2790825" cy="371475"/>
+          <a:off x="4673974" y="746310"/>
+          <a:ext cx="2768413" cy="371475"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
           <a:avLst/>
@@ -136,14 +136,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>168647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>54347</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -154,8 +154,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4724400" y="1457325"/>
-          <a:ext cx="2752725" cy="266700"/>
+          <a:off x="4693024" y="1311647"/>
+          <a:ext cx="2730313" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -225,8 +225,8 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -243,8 +243,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4724400" y="1905000"/>
-          <a:ext cx="2752725" cy="676275"/>
+          <a:off x="4693024" y="1748118"/>
+          <a:ext cx="2730313" cy="833157"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -275,7 +275,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Вычисление дисперсии данного спектра для оценки дисперсии компонент, ограничение амплитуд компонент. </a:t>
+            <a:t>Вычисление дисперсии данного спектра для оценки дисперсии компонент, ограничение амплитуд и скоростей компонент. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1258,8 +1258,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1270,8 +1270,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6296025" y="7591425"/>
-          <a:ext cx="2771775" cy="609600"/>
+          <a:off x="6251201" y="7591425"/>
+          <a:ext cx="2753846" cy="812987"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
           <a:avLst/>
@@ -1340,15 +1340,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>7005</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7005</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>168647</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1360,8 +1360,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6100763" y="1285875"/>
-          <a:ext cx="0" cy="171450"/>
+          <a:off x="6058181" y="1117785"/>
+          <a:ext cx="0" cy="193862"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1390,15 +1390,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>7005</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>54347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7005</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1410,8 +1410,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6100763" y="1724025"/>
-          <a:ext cx="0" cy="180975"/>
+          <a:off x="6058181" y="1578347"/>
+          <a:ext cx="0" cy="169771"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1440,13 +1440,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>7005</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>7005</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -1460,7 +1460,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6100763" y="2581275"/>
+          <a:off x="6058181" y="2581275"/>
           <a:ext cx="0" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1840,13 +1840,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>366713</xdr:colOff>
+      <xdr:colOff>366712</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>366713</xdr:colOff>
+      <xdr:colOff>366712</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -1860,7 +1860,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7681913" y="7258050"/>
+          <a:off x="7628124" y="7258050"/>
           <a:ext cx="0" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2783,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>